<commit_message>
Added Prioroty form PO
</commit_message>
<xml_diff>
--- a/docs/task06/T06_Scrum_Planning_Gruppe_Black_V0.1.xlsx
+++ b/docs/task06/T06_Scrum_Planning_Gruppe_Black_V0.1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henzi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henzi\Desktop\Studium\Semester4\SE\git\ch.bfh.bti7081.s2018.black\docs\task06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0B2609F0-7E74-4578-840A-4BCD5D7DC900}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D94D3D4A-BD15-4A44-9620-1C82A290C480}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="73">
   <si>
     <t>ID</t>
   </si>
@@ -215,6 +215,33 @@
   </si>
   <si>
     <t>Scrum-Master 1. Sprint</t>
+  </si>
+  <si>
+    <t>Im ersten Sprint evt. Spliten</t>
+  </si>
+  <si>
+    <t>Optisches Grundgerüst / Haupt UI</t>
+  </si>
+  <si>
+    <t>1. Sprint</t>
+  </si>
+  <si>
+    <t>Hight</t>
+  </si>
+  <si>
+    <t>Mid</t>
+  </si>
+  <si>
+    <t>Voraussetzung für Notzien</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Superimplemetation: Medikamente</t>
+  </si>
+  <si>
+    <t>Voraussetzung Patientenakte</t>
   </si>
 </sst>
 </file>
@@ -285,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -303,14 +330,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -652,7 +676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -737,10 +761,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,9 +777,10 @@
     <col min="6" max="6" width="13.140625" customWidth="1"/>
     <col min="7" max="7" width="10.140625" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -781,81 +806,136 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="D2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="165" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="D3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="D4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="D5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="D6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="L6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="D7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>62</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" t="s">
+        <v>67</v>
+      </c>
+      <c r="L9" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Sprintplanning for first Sprint.
</commit_message>
<xml_diff>
--- a/docs/task06/T06_Scrum_Planning_Gruppe_Black_V0.1.xlsx
+++ b/docs/task06/T06_Scrum_Planning_Gruppe_Black_V0.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henzi\Desktop\Studium\Semester4\SE\git\ch.bfh.bti7081.s2018.black\docs\task06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D94D3D4A-BD15-4A44-9620-1C82A290C480}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{34133335-9749-4698-AAD7-D4DB37FE3263}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="77">
   <si>
     <t>ID</t>
   </si>
@@ -43,24 +43,6 @@
     <t>high</t>
   </si>
   <si>
-    <t>medium</t>
-  </si>
-  <si>
-    <t>low</t>
-  </si>
-  <si>
-    <t>waiting</t>
-  </si>
-  <si>
-    <t>work in progress</t>
-  </si>
-  <si>
-    <t>done</t>
-  </si>
-  <si>
-    <t>cancelled</t>
-  </si>
-  <si>
     <t>Owner</t>
   </si>
   <si>
@@ -76,36 +58,6 @@
     <t>Effort Actual</t>
   </si>
   <si>
-    <t>Martin</t>
-  </si>
-  <si>
-    <t>Hans</t>
-  </si>
-  <si>
-    <t>Tom</t>
-  </si>
-  <si>
-    <t>Jennifer</t>
-  </si>
-  <si>
-    <t>Database</t>
-  </si>
-  <si>
-    <t>UI, Controller</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>Main Window</t>
-  </si>
-  <si>
-    <t>Patient Model</t>
-  </si>
-  <si>
-    <t>Data model for patient record needs to be created based on standard....</t>
-  </si>
-  <si>
     <t>Effort Plan Original</t>
   </si>
   <si>
@@ -242,6 +194,66 @@
   </si>
   <si>
     <t>Voraussetzung Patientenakte</t>
+  </si>
+  <si>
+    <t>Optisches Grundgerüst / Haupt UI - Interaktionselemente</t>
+  </si>
+  <si>
+    <t>Optisches Grundgerüst / Haupt UI - Darstellung</t>
+  </si>
+  <si>
+    <t>Alle Interaktionselemente des Haupt-UI's erzeugen</t>
+  </si>
+  <si>
+    <t>An Hand der Prototypen, Storyboards und UI-Entwürfen die Interaktionselemente entsprechend platzieren</t>
+  </si>
+  <si>
+    <t>UI, View</t>
+  </si>
+  <si>
+    <t>accepted</t>
+  </si>
+  <si>
+    <t>Haupt UI / Agenda - Schnitstellen</t>
+  </si>
+  <si>
+    <t>Schnittstelle zu Presenter und Model implementieren damit Wechsel auf Agenda-UI möglich wird.</t>
+  </si>
+  <si>
+    <t>Bread-Crumbs - Navigation</t>
+  </si>
+  <si>
+    <t>Damit die Orientierung schon früh gewährleistet werden kann eine sog. Bread-Crumbs-Navigation implementieren. Voraussetzung: Es besteht die Möglichkeit zwischen Agenda und Haupt-UI zu wechseln.</t>
+  </si>
+  <si>
+    <t>UI, View, Presenter, Model, Agenda</t>
+  </si>
+  <si>
+    <t>mid</t>
+  </si>
+  <si>
+    <t>Agenda - Haupt-UI</t>
+  </si>
+  <si>
+    <t>Ein Haupt-UI für die Agenda Implementieren, welche vorbereitet ist für Interationen</t>
+  </si>
+  <si>
+    <t>Agenda, UI</t>
+  </si>
+  <si>
+    <t>Agenda - Kalender</t>
+  </si>
+  <si>
+    <t>Ein Kalender bereitstellen (Recherche Vaadin möglichkeiten Vaadin und Java), bei dem es später ist Termine zu hinterlegen.</t>
+  </si>
+  <si>
+    <t>Agenda - Darstellung</t>
+  </si>
+  <si>
+    <t>Die Benutzeroberfläche so gestalten, dass diese zum Design des Haupt-UI's passt und mit den Entwürfen überein stimmt.</t>
+  </si>
+  <si>
+    <t>Agenda, View</t>
   </si>
 </sst>
 </file>
@@ -312,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -335,6 +347,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -692,66 +710,66 @@
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -763,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,7 +803,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
@@ -794,13 +812,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>4</v>
@@ -811,16 +829,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="105" x14ac:dyDescent="0.25">
@@ -828,13 +846,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="I3" s="2"/>
     </row>
@@ -843,13 +861,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="I4" s="2"/>
     </row>
@@ -858,16 +876,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="120" x14ac:dyDescent="0.25">
@@ -875,19 +893,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="L6" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="75" x14ac:dyDescent="0.25">
@@ -895,16 +913,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="I7" s="2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="105" x14ac:dyDescent="0.25">
@@ -912,16 +930,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -929,13 +947,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="L9" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -946,18 +964,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" customWidth="1"/>
@@ -973,7 +991,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -982,199 +1000,238 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="B2">
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1">
+        <v>4</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="1">
+        <v>4</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="1">
+        <v>5</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" s="1">
+        <v>4</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="1">
+        <v>4</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
-      <c r="J2">
-        <v>2</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1.2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I3">
-        <v>8</v>
-      </c>
-      <c r="J3">
-        <v>6</v>
-      </c>
-      <c r="K3">
+      <c r="I7" s="1">
         <v>4</v>
       </c>
-      <c r="L3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1.3</v>
-      </c>
-      <c r="B4">
+      <c r="L7" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4">
-        <v>16</v>
-      </c>
-      <c r="J4">
-        <v>20</v>
-      </c>
-      <c r="K4">
-        <f>SUM(J4:J4)</f>
-        <v>20</v>
-      </c>
-      <c r="L4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2.1</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5">
+      <c r="C8" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I8" s="1">
         <v>4</v>
       </c>
-      <c r="J5">
-        <v>10</v>
-      </c>
-      <c r="K5">
-        <v>4</v>
-      </c>
-      <c r="L5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6">
-        <v>8</v>
-      </c>
-      <c r="J6">
-        <v>6</v>
-      </c>
-      <c r="K6">
-        <v>5</v>
-      </c>
-      <c r="L6" t="s">
-        <v>9</v>
-      </c>
+      <c r="L8" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1195,16 +1252,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added time estimation to Sprintplanning.
</commit_message>
<xml_diff>
--- a/docs/task06/T06_Scrum_Planning_Gruppe_Black_V0.1.xlsx
+++ b/docs/task06/T06_Scrum_Planning_Gruppe_Black_V0.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henzi\Desktop\Studium\Semester4\SE\git\ch.bfh.bti7081.s2018.black\docs\task06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{34133335-9749-4698-AAD7-D4DB37FE3263}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E5D6FEC6-35A4-462F-AAA3-7C76B57DE00E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="78">
   <si>
     <t>ID</t>
   </si>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t>Agenda, View</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -779,10 +782,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,6 +840,9 @@
       <c r="D2" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="E2" s="1">
+        <v>30</v>
+      </c>
       <c r="I2" s="2" t="s">
         <v>56</v>
       </c>
@@ -854,6 +860,9 @@
       <c r="D3" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="E3">
+        <v>30</v>
+      </c>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:12" ht="165" x14ac:dyDescent="0.25">
@@ -869,6 +878,9 @@
       <c r="D4" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="E4">
+        <v>40</v>
+      </c>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="120" x14ac:dyDescent="0.25">
@@ -884,6 +896,9 @@
       <c r="D5" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
       <c r="I5" s="2" t="s">
         <v>53</v>
       </c>
@@ -901,6 +916,9 @@
       <c r="D6" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="E6">
+        <v>40</v>
+      </c>
       <c r="I6" s="2" t="s">
         <v>48</v>
       </c>
@@ -921,6 +939,9 @@
       <c r="D7" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
       <c r="I7" s="2" t="s">
         <v>55</v>
       </c>
@@ -938,6 +959,9 @@
       <c r="D8" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
       <c r="I8" s="2" t="s">
         <v>55</v>
       </c>
@@ -952,8 +976,20 @@
       <c r="D9" t="s">
         <v>51</v>
       </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
       <c r="L9" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10">
+        <f>SUM(E2:E9)</f>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -967,7 +1003,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,7 +1082,7 @@
         <v>5</v>
       </c>
       <c r="I2" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -1076,7 +1112,7 @@
         <v>5</v>
       </c>
       <c r="I3" s="1">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -1106,7 +1142,7 @@
         <v>5</v>
       </c>
       <c r="I4" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -1136,7 +1172,7 @@
         <v>68</v>
       </c>
       <c r="I5" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -1166,7 +1202,7 @@
         <v>5</v>
       </c>
       <c r="I6" s="1">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -1194,7 +1230,7 @@
         <v>5</v>
       </c>
       <c r="I7" s="1">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>62</v>
@@ -1220,7 +1256,7 @@
         <v>68</v>
       </c>
       <c r="I8" s="1">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>62</v>
@@ -1228,6 +1264,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I9">
+        <f>SUM(I2:I8)</f>
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>